<commit_message>
added table of specifications
</commit_message>
<xml_diff>
--- a/Step4/Step4_Tables.xlsx
+++ b/Step4/Step4_Tables.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB1E76-8FE4-4DFB-B805-094A5CBFCAE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,236 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>Linear Distance</t>
+  </si>
+  <si>
+    <t>Range: 0.5m-3.0m</t>
+  </si>
+  <si>
+    <t>Prevent the robot from colliding with surrounding</t>
+  </si>
+  <si>
+    <t>Response Time: 0.1s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure the robot can respond quickly enough to avoid collisions </t>
+  </si>
+  <si>
+    <t>Sample Rate: &gt;10 Hz</t>
+  </si>
+  <si>
+    <t>Ensure the system receives sensor data at an acceptable rate</t>
+  </si>
+  <si>
+    <t>Magnetic</t>
+  </si>
+  <si>
+    <t>Linearity Error: &lt; 2%</t>
+  </si>
+  <si>
+    <t>Accurately detect the location of the magnetic field from tesseract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field </t>
+  </si>
+  <si>
+    <t>Low Reliability Error</t>
+  </si>
+  <si>
+    <t>Consistently and accurately locate the position of the tesseract</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Resolution: &lt; 1 mG</t>
+  </si>
+  <si>
+    <t>Detect small changes in magnetic field to move toward tesseract</t>
+  </si>
+  <si>
+    <t>Presence and</t>
+  </si>
+  <si>
+    <t>Rise Time: &lt; 0.05s</t>
+  </si>
+  <si>
+    <t>Adjust robot’s direction of travel toward pyramid IR light quickly</t>
+  </si>
+  <si>
+    <t>Direction of</t>
+  </si>
+  <si>
+    <t>Field of View: &gt; 90</t>
+  </si>
+  <si>
+    <t>Increase chances of exposure to pyramid’s IR light</t>
+  </si>
+  <si>
+    <t>IR Light</t>
+  </si>
+  <si>
+    <t>Sample Rate: &gt; 10 Hz</t>
+  </si>
+  <si>
+    <t>Provide system at a sufficiently fast rate</t>
+  </si>
+  <si>
+    <t>Tesseract Detection Sensor Requirements</t>
+  </si>
+  <si>
+    <t>Pyramid Detection Sensor Requirements</t>
+  </si>
+  <si>
+    <t>Wall Detection Sensor Requirements</t>
+  </si>
+  <si>
+    <t>Friction</t>
+  </si>
+  <si>
+    <t>\mu_{friction}: &gt; 0.8</t>
+  </si>
+  <si>
+    <t>A large \mu_{friction} maximizes the power used to move the vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torque </t>
+  </si>
+  <si>
+    <t>Output Torque: &gt; 8 kN.m</t>
+  </si>
+  <si>
+    <t>Approximate power needed to move vehicle at 2 m/s</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Power/Motor: &gt; 40 kW</t>
+  </si>
+  <si>
+    <t>Approximate power needed to move the vehicle</t>
+  </si>
+  <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>Input Torque: &gt; 80 N.m</t>
+  </si>
+  <si>
+    <t>Minimize the complexity of transmission needed for output power</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Effieciency: &gt; 85 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximize the power transferred from the motor to the vehicle </t>
+  </si>
+  <si>
+    <t>Power: &lt; 10 kW</t>
+  </si>
+  <si>
+    <t>Minimize power consumption to leave enough power for movement</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Linearity Error: &lt; 1%</t>
+  </si>
+  <si>
+    <t>Accuracy is needed to manipulate the tesseract and pyramid</t>
+  </si>
+  <si>
+    <t>Torque required to lift pyramid at 1.5 m from frame of vehicle</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Must be able to lift pyramid</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Lift Pyramid high enough to place tesseract underneath</t>
+  </si>
+  <si>
+    <t>Max Load: 2500 kg</t>
+  </si>
+  <si>
+    <t>Stroke Length: 36 in</t>
+  </si>
+  <si>
+    <t>Drivetrain Requirements</t>
+  </si>
+  <si>
+    <t>Powertrain Requirements</t>
+  </si>
+  <si>
+    <t>Max Torque: &gt; 3750N</t>
+  </si>
+  <si>
+    <t>Pyramid Retrieval Requirements</t>
+  </si>
+  <si>
+    <t>Tesseract Retrieval Requirement</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +259,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,12 +267,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +708,296 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A17:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added formetted requirements table
</commit_message>
<xml_diff>
--- a/Step4/Step4_Tables.xlsx
+++ b/Step4/Step4_Tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB1E76-8FE4-4DFB-B805-094A5CBFCAE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E096B52-F5A3-4D91-825A-E0D6E369A0B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,20 +376,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -399,15 +393,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,6 +419,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,279 +717,279 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="3" max="3" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added table of loading and dimensions data for powertrain calcs
</commit_message>
<xml_diff>
--- a/Step4/Step4_Tables.xlsx
+++ b/Step4/Step4_Tables.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA376F3-C179-41B7-9FB8-DA551C46BD1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDE923C-53F2-4FE7-8CB6-21A2C6445418}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2928" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Variable</t>
   </si>
@@ -221,10 +221,22 @@
     <t>3 m/s</t>
   </si>
   <si>
-    <t>Mass</t>
-  </si>
-  <si>
     <t>30 000 kg</t>
+  </si>
+  <si>
+    <t>0.5 m</t>
+  </si>
+  <si>
+    <t>Total Mass</t>
+  </si>
+  <si>
+    <t>Distance to Center of Gravity</t>
+  </si>
+  <si>
+    <t>1.92 m</t>
+  </si>
+  <si>
+    <t>Tread Radius</t>
   </si>
 </sst>
 </file>
@@ -1029,15 +1041,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7EA406-2514-47FF-9BDA-FB47FD1E4EA2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1049,18 +1061,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>